<commit_message>
Addressed various data issues identified by PC.
</commit_message>
<xml_diff>
--- a/dashboard_loader/skills_higher_qual_uploader/skills_higher_qual.xlsx
+++ b/dashboard_loader/skills_higher_qual_uploader/skills_higher_qual.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -237,7 +237,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -266,18 +266,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -299,10 +287,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -330,13 +314,17 @@
   </sheetPr>
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -452,7 +440,9 @@
       <c r="I4" s="6" t="n">
         <v>366</v>
       </c>
-      <c r="J4" s="6"/>
+      <c r="J4" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="K4" s="6" t="n">
         <v>9119</v>
       </c>
@@ -913,320 +903,320 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="n">
+      <c r="A18" s="5" t="n">
         <v>2014</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="9" t="n">
+      <c r="C18" s="6" t="n">
         <v>20578</v>
       </c>
-      <c r="D18" s="9" t="n">
+      <c r="D18" s="6" t="n">
         <v>19128</v>
       </c>
-      <c r="E18" s="9" t="n">
+      <c r="E18" s="6" t="n">
         <v>13374</v>
       </c>
-      <c r="F18" s="9" t="n">
+      <c r="F18" s="6" t="n">
         <v>5710</v>
       </c>
-      <c r="G18" s="9" t="n">
+      <c r="G18" s="6" t="n">
         <v>5896</v>
       </c>
-      <c r="H18" s="9" t="n">
+      <c r="H18" s="6" t="n">
         <v>850</v>
       </c>
-      <c r="I18" s="9" t="n">
+      <c r="I18" s="6" t="n">
         <v>1568</v>
       </c>
-      <c r="J18" s="9" t="n">
+      <c r="J18" s="6" t="n">
         <v>348</v>
       </c>
-      <c r="K18" s="9" t="n">
+      <c r="K18" s="6" t="n">
         <v>67452</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="n">
+      <c r="A19" s="5" t="n">
         <v>2014</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="9" t="n">
+      <c r="C19" s="6" t="n">
         <v>3184</v>
       </c>
-      <c r="D19" s="9" t="n">
+      <c r="D19" s="6" t="n">
         <v>4010</v>
       </c>
-      <c r="E19" s="9" t="n">
+      <c r="E19" s="6" t="n">
         <v>843</v>
       </c>
-      <c r="F19" s="9" t="n">
+      <c r="F19" s="6" t="n">
         <v>884</v>
       </c>
-      <c r="G19" s="9" t="n">
+      <c r="G19" s="6" t="n">
         <v>928</v>
       </c>
-      <c r="H19" s="9" t="n">
+      <c r="H19" s="6" t="n">
         <v>127</v>
       </c>
-      <c r="I19" s="9" t="n">
+      <c r="I19" s="6" t="n">
         <v>434</v>
       </c>
-      <c r="J19" s="9" t="n">
+      <c r="J19" s="6" t="n">
         <v>29</v>
       </c>
-      <c r="K19" s="9" t="n">
+      <c r="K19" s="6" t="n">
         <v>10439</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="n">
+      <c r="A20" s="5" t="n">
         <v>2014</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="9" t="n">
+      <c r="C20" s="6" t="n">
         <v>23762</v>
       </c>
-      <c r="D20" s="9" t="n">
+      <c r="D20" s="6" t="n">
         <v>23138</v>
       </c>
-      <c r="E20" s="9" t="n">
+      <c r="E20" s="6" t="n">
         <v>14217</v>
       </c>
-      <c r="F20" s="9" t="n">
+      <c r="F20" s="6" t="n">
         <v>6594</v>
       </c>
-      <c r="G20" s="9" t="n">
+      <c r="G20" s="6" t="n">
         <v>6824</v>
       </c>
-      <c r="H20" s="9" t="n">
+      <c r="H20" s="6" t="n">
         <v>977</v>
       </c>
-      <c r="I20" s="9" t="n">
+      <c r="I20" s="6" t="n">
         <v>2002</v>
       </c>
-      <c r="J20" s="9" t="n">
+      <c r="J20" s="6" t="n">
         <v>377</v>
       </c>
-      <c r="K20" s="9" t="n">
+      <c r="K20" s="6" t="n">
         <v>77891</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="n">
+      <c r="A21" s="5" t="n">
         <v>2015</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="9" t="n">
+      <c r="C21" s="6" t="n">
         <v>15062</v>
       </c>
-      <c r="D21" s="9" t="n">
+      <c r="D21" s="6" t="n">
         <v>19857</v>
       </c>
-      <c r="E21" s="9" t="n">
+      <c r="E21" s="6" t="n">
         <v>9355</v>
       </c>
-      <c r="F21" s="9" t="n">
+      <c r="F21" s="6" t="n">
         <v>5788</v>
       </c>
-      <c r="G21" s="9" t="n">
+      <c r="G21" s="6" t="n">
         <v>3742</v>
       </c>
-      <c r="H21" s="9" t="n">
+      <c r="H21" s="6" t="n">
         <v>669</v>
       </c>
-      <c r="I21" s="9" t="n">
+      <c r="I21" s="6" t="n">
         <v>1537</v>
       </c>
-      <c r="J21" s="9" t="n">
+      <c r="J21" s="6" t="n">
         <v>244</v>
       </c>
-      <c r="K21" s="9" t="n">
+      <c r="K21" s="6" t="n">
         <v>56254</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="n">
+      <c r="A22" s="5" t="n">
         <v>2015</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="9" t="n">
+      <c r="C22" s="6" t="n">
         <v>1794</v>
       </c>
-      <c r="D22" s="9" t="n">
+      <c r="D22" s="6" t="n">
         <v>4046</v>
       </c>
-      <c r="E22" s="9" t="n">
+      <c r="E22" s="6" t="n">
         <v>460</v>
       </c>
-      <c r="F22" s="9" t="n">
+      <c r="F22" s="6" t="n">
         <v>1002</v>
       </c>
-      <c r="G22" s="9" t="n">
+      <c r="G22" s="6" t="n">
         <v>770</v>
       </c>
-      <c r="H22" s="9" t="n">
+      <c r="H22" s="6" t="n">
         <v>110</v>
       </c>
-      <c r="I22" s="9" t="n">
+      <c r="I22" s="6" t="n">
         <v>298</v>
       </c>
-      <c r="J22" s="9" t="n">
+      <c r="J22" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="K22" s="9" t="n">
+      <c r="K22" s="6" t="n">
         <v>8498</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="n">
+      <c r="A23" s="5" t="n">
         <v>2015</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="9" t="n">
+      <c r="C23" s="6" t="n">
         <v>16856</v>
       </c>
-      <c r="D23" s="9" t="n">
+      <c r="D23" s="6" t="n">
         <v>23903</v>
       </c>
-      <c r="E23" s="9" t="n">
+      <c r="E23" s="6" t="n">
         <v>9815</v>
       </c>
-      <c r="F23" s="9" t="n">
+      <c r="F23" s="6" t="n">
         <v>6790</v>
       </c>
-      <c r="G23" s="9" t="n">
+      <c r="G23" s="6" t="n">
         <v>4512</v>
       </c>
-      <c r="H23" s="9" t="n">
+      <c r="H23" s="6" t="n">
         <v>779</v>
       </c>
-      <c r="I23" s="9" t="n">
+      <c r="I23" s="6" t="n">
         <v>1835</v>
       </c>
-      <c r="J23" s="9" t="n">
+      <c r="J23" s="6" t="n">
         <v>262</v>
       </c>
-      <c r="K23" s="9" t="n">
+      <c r="K23" s="6" t="n">
         <v>64752</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="n">
+      <c r="A24" s="5" t="n">
         <v>2016</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="9" t="n">
+      <c r="C24" s="6" t="n">
         <v>13060</v>
       </c>
-      <c r="D24" s="9" t="n">
+      <c r="D24" s="6" t="n">
         <v>17815</v>
       </c>
-      <c r="E24" s="9" t="n">
+      <c r="E24" s="6" t="n">
         <v>9873</v>
       </c>
-      <c r="F24" s="9" t="n">
+      <c r="F24" s="6" t="n">
         <v>4988</v>
       </c>
-      <c r="G24" s="9" t="n">
+      <c r="G24" s="6" t="n">
         <v>3171</v>
       </c>
-      <c r="H24" s="9" t="n">
+      <c r="H24" s="6" t="n">
         <v>708</v>
       </c>
-      <c r="I24" s="9" t="n">
+      <c r="I24" s="6" t="n">
         <v>1365</v>
       </c>
-      <c r="J24" s="9" t="n">
+      <c r="J24" s="6" t="n">
         <v>337</v>
       </c>
-      <c r="K24" s="9" t="n">
+      <c r="K24" s="6" t="n">
         <v>51317</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="n">
+      <c r="A25" s="5" t="n">
         <v>2016</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="9" t="n">
+      <c r="C25" s="6" t="n">
         <v>1191</v>
       </c>
-      <c r="D25" s="9" t="n">
+      <c r="D25" s="6" t="n">
         <v>3225</v>
       </c>
-      <c r="E25" s="9" t="n">
+      <c r="E25" s="6" t="n">
         <v>310</v>
       </c>
-      <c r="F25" s="9" t="n">
+      <c r="F25" s="6" t="n">
         <v>551</v>
       </c>
-      <c r="G25" s="9" t="n">
+      <c r="G25" s="6" t="n">
         <v>583</v>
       </c>
-      <c r="H25" s="9" t="n">
+      <c r="H25" s="6" t="n">
         <v>78</v>
       </c>
-      <c r="I25" s="9" t="n">
+      <c r="I25" s="6" t="n">
         <v>245</v>
       </c>
-      <c r="J25" s="9" t="n">
+      <c r="J25" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="K25" s="9" t="n">
+      <c r="K25" s="6" t="n">
         <v>6211</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="n">
+      <c r="A26" s="5" t="n">
         <v>2016</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="9" t="n">
+      <c r="C26" s="6" t="n">
         <v>14251</v>
       </c>
-      <c r="D26" s="9" t="n">
+      <c r="D26" s="6" t="n">
         <v>21040</v>
       </c>
-      <c r="E26" s="9" t="n">
+      <c r="E26" s="6" t="n">
         <v>10183</v>
       </c>
-      <c r="F26" s="9" t="n">
+      <c r="F26" s="6" t="n">
         <v>5539</v>
       </c>
-      <c r="G26" s="9" t="n">
+      <c r="G26" s="6" t="n">
         <v>3754</v>
       </c>
-      <c r="H26" s="9" t="n">
+      <c r="H26" s="6" t="n">
         <v>786</v>
       </c>
-      <c r="I26" s="9" t="n">
+      <c r="I26" s="6" t="n">
         <v>1610</v>
       </c>
-      <c r="J26" s="9" t="n">
+      <c r="J26" s="6" t="n">
         <v>365</v>
       </c>
-      <c r="K26" s="9" t="n">
+      <c r="K26" s="6" t="n">
         <v>57528</v>
       </c>
-      <c r="L26" s="10"/>
+      <c r="L26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="n">
@@ -1235,15 +1225,15 @@
       <c r="B27" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11" t="n">
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8" t="n">
         <v>107948</v>
       </c>
     </row>
@@ -1265,21 +1255,22 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="132.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1287,7 +1278,7 @@
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1295,7 +1286,7 @@
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1303,7 +1294,7 @@
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="14" t="n">
+      <c r="B4" s="11" t="n">
         <v>2016</v>
       </c>
     </row>
@@ -1311,13 +1302,13 @@
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1325,19 +1316,19 @@
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="13" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1345,7 +1336,7 @@
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1353,7 +1344,7 @@
       <c r="A11" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="13" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>